<commit_message>
fixed amount of worker issue
- separate between make table, get constraints from google form, and automate the schedule assignment.
</commit_message>
<xml_diff>
--- a/automate/תבנית סידור.xlsx
+++ b/automate/תבנית סידור.xlsx
@@ -621,7 +621,7 @@
     <row r="1">
       <c r="A1" s="23" t="inlineStr">
         <is>
-          <t>סידור עבודה צוות עדי</t>
+          <t>s</t>
         </is>
       </c>
       <c r="B1" s="20" t="n"/>
@@ -730,17 +730,27 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Worker 1</t>
+          <t>אוראל</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>b</t>
+          <t>f</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>b.c</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>b</t>
+          <t>f</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>a.b.c</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
@@ -762,13 +772,13 @@
         <v>6</v>
       </c>
       <c r="U2" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="19" t="inlineStr">
         <is>
-          <t xml:space="preserve">עמדה כניסה </t>
+          <t>עמדה 1</t>
         </is>
       </c>
       <c r="B3" s="20" t="n"/>
@@ -780,34 +790,34 @@
       <c r="H3" s="21" t="n"/>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Worker 2</t>
+          <t>זיו שהינו</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>c</t>
+          <t>f</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>a.b.c</t>
+          <t>b.c</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
+          <t>f</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>a.b.c</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
           <t>a</t>
         </is>
       </c>
-      <c r="P3" t="inlineStr">
-        <is>
-          <t>c</t>
-        </is>
-      </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>a.b.c</t>
-        </is>
-      </c>
       <c r="R3" t="inlineStr">
         <is>
           <t>a.b.c</t>
@@ -815,14 +825,14 @@
       </c>
       <c r="S3" t="inlineStr">
         <is>
-          <t>a.b.c</t>
+          <t>a.b</t>
         </is>
       </c>
       <c r="T3" t="n">
         <v>6</v>
       </c>
       <c r="U3" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4">
@@ -840,32 +850,32 @@
       <c r="H4" s="7" t="n"/>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Worker 3</t>
-        </is>
-      </c>
-      <c r="L4" s="25" t="inlineStr">
-        <is>
-          <t xml:space="preserve">מבחנים </t>
+          <t>רוני</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>b</t>
+          <t>f</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>b.c</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>c</t>
+          <t>f</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
+          <t>a.b.c</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
           <t>a</t>
-        </is>
-      </c>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t>c</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
@@ -882,7 +892,7 @@
         <v>6</v>
       </c>
       <c r="U4" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">
@@ -900,49 +910,29 @@
       <c r="H5" s="7" t="n"/>
       <c r="J5" t="inlineStr">
         <is>
-          <t>Worker 4</t>
+          <t>יניב שטיינר</t>
+        </is>
+      </c>
+      <c r="L5" s="25" t="inlineStr">
+        <is>
+          <t>חתונה</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>b.c</t>
+          <t>a</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>a.b.c</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
           <t>a</t>
-        </is>
-      </c>
-      <c r="P5" t="inlineStr">
-        <is>
-          <t>b.c</t>
-        </is>
-      </c>
-      <c r="Q5" t="inlineStr">
-        <is>
-          <t>a.b.c</t>
-        </is>
-      </c>
-      <c r="R5" t="inlineStr">
-        <is>
-          <t>a.b.c</t>
-        </is>
-      </c>
-      <c r="S5" t="inlineStr">
-        <is>
-          <t>a.b.c</t>
         </is>
       </c>
       <c r="T5" t="n">
         <v>6</v>
       </c>
       <c r="U5" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -960,45 +950,55 @@
       <c r="H6" s="5" t="n"/>
       <c r="J6" t="inlineStr">
         <is>
-          <t>Worker 7</t>
+          <t>אור</t>
+        </is>
+      </c>
+      <c r="L6" s="25" t="inlineStr">
+        <is>
+          <t>חתונה ברביעי</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
+          <t>a.b.c</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>a.b.c</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>a.b.c</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>b.c</t>
+        </is>
+      </c>
+      <c r="S6" t="inlineStr">
+        <is>
           <t>a.c</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>a.b.c</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>a.b.c</t>
-        </is>
-      </c>
-      <c r="P6" t="inlineStr">
-        <is>
-          <t>a.c</t>
-        </is>
-      </c>
-      <c r="Q6" t="inlineStr">
-        <is>
-          <t>a.b.c</t>
         </is>
       </c>
       <c r="T6" t="n">
         <v>6</v>
       </c>
       <c r="U6" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="19" t="inlineStr">
         <is>
-          <t>עמדה אחורית</t>
+          <t>עמדה 2</t>
         </is>
       </c>
       <c r="B7" s="20" t="n"/>
@@ -1010,7 +1010,17 @@
       <c r="H7" s="21" t="n"/>
       <c r="J7" t="inlineStr">
         <is>
-          <t>Worker 6</t>
+          <t>שבת</t>
+        </is>
+      </c>
+      <c r="L7" s="25" t="inlineStr">
+        <is>
+          <t>עד 4 משמרות לבינתיים 🫡</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>a.b.c</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
@@ -1020,34 +1030,34 @@
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>a.b.c</t>
+          <t>a</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>a.b</t>
+          <t>b.c</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>b.c</t>
+          <t>a.b.c</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
         <is>
-          <t>a.c</t>
+          <t>a.b.c</t>
         </is>
       </c>
       <c r="S7" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>a.b.c</t>
         </is>
       </c>
       <c r="T7" t="n">
         <v>6</v>
       </c>
       <c r="U7" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8">
@@ -1065,29 +1075,19 @@
       <c r="H8" s="7" t="n"/>
       <c r="J8" t="inlineStr">
         <is>
-          <t>Worker 5</t>
-        </is>
-      </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>a.b.c</t>
-        </is>
-      </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>a.b.c</t>
+          <t>עמית בלסן</t>
         </is>
       </c>
       <c r="O8" t="inlineStr">
         <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
           <t>a.c</t>
         </is>
       </c>
-      <c r="P8" t="inlineStr">
-        <is>
-          <t>a.c</t>
-        </is>
-      </c>
       <c r="Q8" t="inlineStr">
         <is>
           <t>a.b.c</t>
@@ -1095,19 +1095,19 @@
       </c>
       <c r="R8" t="inlineStr">
         <is>
-          <t>a.b.c</t>
+          <t>a</t>
         </is>
       </c>
       <c r="S8" t="inlineStr">
         <is>
-          <t>a.b.c</t>
+          <t>c</t>
         </is>
       </c>
       <c r="T8" t="n">
         <v>6</v>
       </c>
       <c r="U8" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9">
@@ -1123,10 +1123,53 @@
       <c r="F9" s="6" t="n"/>
       <c r="G9" s="7" t="n"/>
       <c r="H9" s="7" t="n"/>
-      <c r="J9" s="24" t="inlineStr">
-        <is>
-          <t>תגבור</t>
-        </is>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>אמור</t>
+        </is>
+      </c>
+      <c r="L9" s="25" t="inlineStr">
+        <is>
+          <t>חינה בשלישי בערב. 
+אם אפשר בלי : (b)-(b) בשישי שבת. 
+ומזל טוב לשטיינר</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>a.b</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>b.c</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>a.b.c</t>
+        </is>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>a.b.c</t>
+        </is>
+      </c>
+      <c r="S9" t="inlineStr">
+        <is>
+          <t>a.b</t>
+        </is>
+      </c>
+      <c r="T9" t="n">
+        <v>6</v>
+      </c>
+      <c r="U9" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="10">
@@ -1142,6 +1185,11 @@
       <c r="F10" s="13" t="n"/>
       <c r="G10" s="7" t="n"/>
       <c r="H10" s="5" t="n"/>
+      <c r="J10" s="24" t="inlineStr">
+        <is>
+          <t>תגבור</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="22" t="inlineStr">

</xml_diff>